<commit_message>
adding sheet param to xlsx2tsv and add test
</commit_message>
<xml_diff>
--- a/tests/testthat/example_xlsx.xlsx
+++ b/tests/testthat/example_xlsx.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pgc92/Desktop/nvutils/nvutils/tests/testthat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pgc92/local/opt/nvutils/tests/testthat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F495E078-63BC-4148-8001-0323E6BE8CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61EDEF0-C9BC-AB4F-8F0D-4701F70E5AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foo" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>foo</t>
   </si>
@@ -45,11 +46,17 @@
   <si>
     <t>orange</t>
   </si>
+  <si>
+    <t>sheet2</t>
+  </si>
+  <si>
+    <t>sheet2_col2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -883,10 +890,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -956,4 +963,27 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44FF2A1-F0EA-C640-A279-59040C131FF9}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding sep.names and detectDates params to xlsx2tsv()
</commit_message>
<xml_diff>
--- a/tests/testthat/example_xlsx.xlsx
+++ b/tests/testthat/example_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pgc92/local/opt/nvutils/tests/testthat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\pgc92\local\opt\nvutils\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61EDEF0-C9BC-AB4F-8F0D-4701F70E5AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28DEE61-5421-4BBC-B134-BC2FED004EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2760" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foo" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>foo</t>
   </si>
@@ -29,9 +29,6 @@
     <t>bar</t>
   </si>
   <si>
-    <t>baz</t>
-  </si>
-  <si>
     <t>red</t>
   </si>
   <si>
@@ -51,6 +48,18 @@
   </si>
   <si>
     <t>sheet2_col2</t>
+  </si>
+  <si>
+    <t>count of  files</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>date.now</t>
+  </si>
+  <si>
+    <t>baz&gt;qux</t>
   </si>
 </sst>
 </file>
@@ -534,8 +543,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -595,9 +622,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -635,7 +662,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -741,7 +768,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -883,7 +910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -891,72 +918,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>170.1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43532</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.28689477956338882</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="6">
+        <v>16808</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>170.1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>10.9</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43800</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.73915932966927533</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10.9</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>199.2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43160</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.35506826454786744</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="E4" s="6">
+        <v>18630</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>199.2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>229</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45337</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.98924351240489949</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
+      <c r="E5" s="6"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>229</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="B6" s="5">
+        <v>45002</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.98532309769208004</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
+      <c r="E6" s="6">
         <v>0</v>
       </c>
     </row>
@@ -969,18 +1043,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44FF2A1-F0EA-C640-A279-59040C131FF9}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
R/xlsx2tsv.R     Replace readr::write_tsv with data.table::fwrite in xlsx2tsv() and updated tests     - fwrite is faster and has better NA handling     - keep literal "NA" on read and write true blanks (without quotes)     - read.xlsx() - add na.strings = character(0) to prevent converting "NA" text to missing     - fwrite() - add quote = FALSE to avoid outputting "" for empty cells
R/tsv2xlsx.R
    Refactor tsv2xlsx to use data.table::fread and replace readr::read_tsv
    - Default to colClasses = 'character' to preserve text (incl. leading zeros)
    - Set na.strings = NULL by default to keep '' as '' and 'NA' as literal text
    - Deprecate show_col_types and guess_max; add warnings

scripts tsv2xlsx.R and xlsx2tsv.R
    updated so they are compatible with the switch to fread/fwrite
</commit_message>
<xml_diff>
--- a/tests/testthat/example_xlsx.xlsx
+++ b/tests/testthat/example_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\pgc92\local\opt\nvutils\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pgc92/local/opt/nvutils/tests/testthat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28DEE61-5421-4BBC-B134-BC2FED004EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4A0ACB-096E-C84F-AE58-C1A0B8A1974E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2760" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foo" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>foo</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>black</t>
-  </si>
-  <si>
-    <t>orange</t>
   </si>
   <si>
     <t>sheet2</t>
@@ -920,38 +917,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="27" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="27" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>170.1</v>
       </c>
@@ -968,7 +965,7 @@
         <v>16808</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>10.9</v>
       </c>
@@ -982,10 +979,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>199.2</v>
       </c>
@@ -1002,7 +999,7 @@
         <v>18630</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>229</v>
       </c>
@@ -1017,7 +1014,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>16.399999999999999</v>
       </c>
@@ -1026,9 +1023,6 @@
       </c>
       <c r="C6" s="1">
         <v>0.98532309769208004</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
@@ -1047,14 +1041,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>